<commit_message>
minor update to narc file
</commit_message>
<xml_diff>
--- a/data/09d-narcsissus.xlsx
+++ b/data/09d-narcsissus.xlsx
@@ -387,8 +387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:AG32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:BJ1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1907,5 +1907,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="F6 G6:M6" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>